<commit_message>
code change final demo
</commit_message>
<xml_diff>
--- a/Data/LeadsExport.xlsx
+++ b/Data/LeadsExport.xlsx
@@ -1685,10 +1685,10 @@
       <c r="V2" s="4"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y2" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>61</v>
@@ -1789,10 +1789,10 @@
       <c r="V3" s="4"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y3" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z3" s="4" t="s">
         <v>61</v>
@@ -1893,10 +1893,10 @@
       <c r="V4" s="4"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y4" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z4" s="4" t="s">
         <v>61</v>
@@ -1997,10 +1997,10 @@
       <c r="V5" s="4"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y5" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>61</v>
@@ -2101,10 +2101,10 @@
       <c r="V6" s="4"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y6" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z6" s="4" t="s">
         <v>61</v>
@@ -2209,10 +2209,10 @@
       <c r="V7" s="4"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y7" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z7" s="4" t="s">
         <v>61</v>
@@ -2315,10 +2315,10 @@
       <c r="V8" s="4"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y8" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>61</v>
@@ -2421,10 +2421,10 @@
         <v>44090.26538194444583</v>
       </c>
       <c r="X9" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y9" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z9" s="4" t="s">
         <v>61</v>
@@ -2525,10 +2525,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y10" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z10" s="4" t="s">
         <v>61</v>
@@ -2629,10 +2629,10 @@
       <c r="V11" s="4"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y11" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z11" s="4" t="s">
         <v>61</v>
@@ -2733,10 +2733,10 @@
       <c r="V12" s="4"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y12" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z12" s="4" t="s">
         <v>61</v>
@@ -2835,10 +2835,10 @@
       <c r="V13" s="4"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y13" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z13" s="4" t="s">
         <v>61</v>
@@ -2941,10 +2941,10 @@
         <v>44284.38123842592904</v>
       </c>
       <c r="X14" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y14" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z14" s="4" t="s">
         <v>61</v>
@@ -3045,10 +3045,10 @@
       <c r="V15" s="4"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y15" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>61</v>
@@ -3149,10 +3149,10 @@
       <c r="V16" s="4"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y16" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z16" s="4" t="s">
         <v>61</v>
@@ -3253,10 +3253,10 @@
       <c r="V17" s="4"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y17" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z17" s="4" t="s">
         <v>61</v>
@@ -3359,10 +3359,10 @@
         <v>44089.37105324074219</v>
       </c>
       <c r="X18" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y18" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z18" s="4" t="s">
         <v>61</v>
@@ -3465,10 +3465,10 @@
         <v>44435.29143518518686</v>
       </c>
       <c r="X19" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y19" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z19" s="4" t="s">
         <v>61</v>
@@ -3567,10 +3567,10 @@
       <c r="V20" s="4"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y20" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z20" s="4" t="s">
         <v>61</v>
@@ -3671,10 +3671,10 @@
       <c r="V21" s="4"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Y21" s="5">
-        <v>46065.91682870370278</v>
+        <v>46066.33349537036702</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>61</v>

</xml_diff>